<commit_message>
Biểu diễn dữ liệu từ trình soạn thảo văn bản
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/procedure.xlsx
+++ b/Hethongquanlylab/wwwroot/data/procedure.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>id</t>
   </si>
@@ -88,20 +88,33 @@
     <t>Quy trình đào tạo</t>
   </si>
   <si>
+    <t>09/09/2022</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Hello&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>1233</t>
   </si>
   <si>
-    <t>09/09/2022</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Hello&lt;/strong&gt;&lt;/p&gt;</t>
+    <t xml:space="preserve">&lt;p&gt;&lt;strong style="font-size: 18px;"&gt;Đây là quy trình đào tạo&lt;/strong&gt;&lt;/p&gt;&lt;table style="border-collapse:collapse;width: 100%;"&gt;&lt;tbody&gt;_x000D_
+&lt;tr&gt;_x000D_
+_x0009_&lt;td style="width: 50%;"&gt;Hello&lt;/td&gt;_x000D_
+_x0009_&lt;td style="width: 50%;"&gt;Test&lt;/td&gt;&lt;/tr&gt;_x000D_
+&lt;tr&gt;_x000D_
+_x0009_&lt;td style="width: 50%;"&gt;&lt;br&gt;&lt;/td&gt;_x000D_
+_x0009_&lt;td style="width: 50%;"&gt;&lt;br&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;</t>
+  </si>
+  <si>
+    <t>123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,11 +141,11 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
+    <xf numFmtId="14" applyNumberFormat="1" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,7 +460,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B357BE-472C-4729-B72D-D70006B2101F}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
@@ -461,148 +474,169 @@
     <col min="5" max="5" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
+    <row r="1">
+      <c r="A1" s="0" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="0" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A2">
+    <row r="2">
+      <c r="A2" s="0">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="0" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>44562</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="0">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A3">
+    <row r="3">
+      <c r="A3" s="0">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="0" t="s">
         <v>9</v>
       </c>
       <c r="C3" s="1">
         <v>44563</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="0">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A4">
+    <row r="4">
+      <c r="A4" s="0">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="1">
         <v>44564</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="0">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A5">
+    <row r="5">
+      <c r="A5" s="0">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="0" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="1">
         <v>44565</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E5" t="s">
+      <c r="E5" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="0">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A6">
+    <row r="6">
+      <c r="A6" s="0">
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="0" t="s">
         <v>15</v>
       </c>
       <c r="C6" s="1">
         <v>44566</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="E6" t="s">
+      <c r="E6" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="0">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A7">
+    <row r="7">
+      <c r="A7" s="0">
         <v>7</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="0" t="s">
         <v>16</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F7" t="s">
-        <v>17</v>
+      <c r="F8" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Quy trình giao diện
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/procedure.xlsx
+++ b/Hethongquanlylab/wwwroot/data/procedure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AB6417-240F-4E8D-88FD-825B10C5D920}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2602F8-1493-4E82-9C9C-71660C8D2433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1688" yWindow="3427" windowWidth="14400" windowHeight="7373" xr2:uid="{C9AB2BF0-DA74-4C36-9550-9AB44C18DC50}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{C9AB2BF0-DA74-4C36-9550-9AB44C18DC50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>id</t>
   </si>
@@ -43,12 +43,24 @@
     <t>Tên dự án</t>
   </si>
   <si>
+    <t>Đơn vị</t>
+  </si>
+  <si>
     <t>Ngày bắt đầu</t>
   </si>
   <si>
     <t>Nội dung</t>
   </si>
   <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>V2</t>
+  </si>
+  <si>
+    <t>V3</t>
+  </si>
+  <si>
     <t>Tình trạng</t>
   </si>
   <si>
@@ -58,7 +70,13 @@
     <t>Quy trình tuyển 5.3</t>
   </si>
   <si>
+    <t>BanNhanSu</t>
+  </si>
+  <si>
     <t>Chi tiết nội dung</t>
+  </si>
+  <si>
+    <t>False</t>
   </si>
   <si>
     <t>Đã duyệt</t>
@@ -107,6 +125,12 @@
   </si>
   <si>
     <t>123</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong style="font-size: 11px;"&gt;&lt;em style="font-size: 30px; color: rgb(255, 0, 0);"&gt;adsadsadsa&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
 </sst>
 </file>
@@ -460,18 +484,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B357BE-472C-4729-B72D-D70006B2101F}">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="26.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.53125" customWidth="1"/>
-    <col min="4" max="4" width="17.53125" customWidth="1"/>
-    <col min="5" max="5" width="13.19921875" customWidth="1"/>
+    <col min="2" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" customWidth="1"/>
+    <col min="5" max="5" width="17.53125" customWidth="1"/>
+    <col min="9" max="9" width="13.19921875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -493,24 +517,48 @@
       <c r="F1" s="0" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1">
         <v>44562</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="E2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" s="0">
+        <v>12</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0">
         <v>1</v>
       </c>
     </row>
@@ -519,18 +567,30 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="1">
+        <v>15</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="1">
         <v>44563</v>
       </c>
-      <c r="D3" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="E3" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" s="0">
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="0">
         <v>2</v>
       </c>
     </row>
@@ -539,18 +599,30 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1">
+      <c r="D4" s="1">
         <v>44564</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>7</v>
       </c>
       <c r="E4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="0">
+      <c r="F4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J4" s="0">
         <v>3</v>
       </c>
     </row>
@@ -559,18 +631,30 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1">
+        <v>19</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="1">
         <v>44565</v>
       </c>
-      <c r="D5" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="0">
+        <v>12</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J5" s="0">
         <v>4</v>
       </c>
     </row>
@@ -579,18 +663,30 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="1">
+        <v>21</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="1">
         <v>44566</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>7</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F6" s="0">
+        <v>12</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="J6" s="0">
         <v>5</v>
       </c>
     </row>
@@ -599,19 +695,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D7" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="F7" s="0" t="s">
-        <v>19</v>
+      <c r="J7" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="8">
@@ -619,19 +727,63 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>21</v>
+        <v>13</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -817,18 +969,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -850,14 +1002,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC5E854-D858-439B-BCEB-E443416E5990}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9ACA1CD9-D4DF-4A7B-8ECE-9D8D5209CA6B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -871,4 +1015,12 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC5E854-D858-439B-BCEB-E443416E5990}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Gửi duyêt + gửi mail (Đang để mail cố định nên chỉ dùng đc tại 1 máy)
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/procedure.xlsx
+++ b/Hethongquanlylab/wwwroot/data/procedure.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2602F8-1493-4E82-9C9C-71660C8D2433}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789E380-2636-4AC5-A249-98583EB3E4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{C9AB2BF0-DA74-4C36-9550-9AB44C18DC50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="BanNhanSu" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
   <extLst>
@@ -67,46 +68,55 @@
     <t>Link</t>
   </si>
   <si>
-    <t>Quy trình tuyển 5.3</t>
+    <t>Nguyễn Văn Bình</t>
+  </si>
+  <si>
+    <t>BanDaoTao</t>
+  </si>
+  <si>
+    <t>10/09/2022</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Quy trình gặp mặt&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Chưa duyệt</t>
+  </si>
+  <si>
+    <t>fjdfhjdfhajf</t>
+  </si>
+  <si>
+    <t>Quy trình Offline các PT</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;đây là quy trình offline PT&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>đâf</t>
+  </si>
+  <si>
+    <t>Quy trình Offline PT</t>
+  </si>
+  <si>
+    <t>&lt;p style="text-align: center;"&gt;&lt;span style="background-color: rgb(255, 0, 0);"&gt;Đây là quy trình quan trọng&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>dfjadfjdsaf</t>
+  </si>
+  <si>
+    <t>Quy trình Offline Lab</t>
+  </si>
+  <si>
+    <t>&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0);"&gt;Đây là quy trình rất quan trọng&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>BanNhanSu</t>
   </si>
   <si>
-    <t>11/09/2022</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Cần thêm thành viên tham gia&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>Chưa duyệt</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Đề án cuộc thi NCKH</t>
-  </si>
-  <si>
-    <t>Chi tiết nội dung</t>
-  </si>
-  <si>
-    <t>False</t>
-  </si>
-  <si>
-    <t>Trả lại</t>
-  </si>
-  <si>
-    <t>Đề án cuộc thi sáng tạo trẻ</t>
-  </si>
-  <si>
-    <t>Quy trình gặp 1-1</t>
-  </si>
-  <si>
-    <t>Chờ duyệt</t>
-  </si>
-  <si>
-    <t>Quy trình tuyển thành viên ban</t>
+    <t>&lt;p&gt;Ngày 20/8/2022, Lab thầy Sinh tổ chức offline Lab tại trụ sở Tư Đình, Long Biên, Hà Nội&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>2hfsdjfhjkadfhads</t>
   </si>
   <si>
     <t>Quy trình đào tạo</t>
@@ -115,10 +125,10 @@
     <t>09/09/2022</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong&gt;Hello&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>1233</t>
+    <t>&lt;p&gt;&lt;strong style="font-size: 11px;"&gt;&lt;em style="font-size: 30px; color: rgb(255, 0, 0);"&gt;adsadsadsa&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1234</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;p&gt;&lt;strong style="font-size: 18px;"&gt;Đây là quy trình đào tạo&lt;/strong&gt;&lt;/p&gt;&lt;table style="border-collapse:collapse;width: 100%;"&gt;&lt;tbody&gt;_x000D_
@@ -130,58 +140,49 @@
 _x0009_&lt;td style="width: 50%;"&gt;&lt;br&gt;&lt;/td&gt;&lt;/tr&gt;&lt;/tbody&gt;&lt;/table&gt;</t>
   </si>
   <si>
+    <t>False</t>
+  </si>
+  <si>
     <t>123</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;strong style="font-size: 11px;"&gt;&lt;em style="font-size: 30px; color: rgb(255, 0, 0);"&gt;adsadsadsa&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>1234</t>
-  </si>
-  <si>
-    <t>Quy trình Offline Lab</t>
-  </si>
-  <si>
-    <t>10/09/2022</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ngày 20/8/2022, Lab thầy Sinh tổ chức offline Lab tại trụ sở Tư Đình, Long Biên, Hà Nội&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>2hfsdjfhjkadfhads</t>
-  </si>
-  <si>
-    <t>BanDaoTao</t>
-  </si>
-  <si>
-    <t>&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0);"&gt;Đây là quy trình rất quan trọng&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>fjdfhjdfhajf</t>
-  </si>
-  <si>
-    <t>Quy trình Offline PT</t>
-  </si>
-  <si>
-    <t>&lt;p style="text-align: center;"&gt;&lt;span style="background-color: rgb(255, 0, 0);"&gt;Đây là quy trình quan trọng&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>dfjadfjdsaf</t>
-  </si>
-  <si>
-    <t>Quy trình Offline các PT</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;đây là quy trình offline PT&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>đâf</t>
-  </si>
-  <si>
-    <t>Nguyễn Văn Bình</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Quy trình gặp mặt&lt;/p&gt;</t>
+    <t>&lt;p&gt;&lt;strong&gt;Hello&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1233</t>
+  </si>
+  <si>
+    <t>Quy trình tuyển thành viên ban</t>
+  </si>
+  <si>
+    <t>Chi tiết nội dung</t>
+  </si>
+  <si>
+    <t>Chờ duyệt</t>
+  </si>
+  <si>
+    <t>Quy trình gặp 1-1</t>
+  </si>
+  <si>
+    <t>Đề án cuộc thi sáng tạo trẻ</t>
+  </si>
+  <si>
+    <t>Đề án cuộc thi NCKH</t>
+  </si>
+  <si>
+    <t>Trả lại</t>
+  </si>
+  <si>
+    <t>Quy trình tuyển 5.3t5345678</t>
+  </si>
+  <si>
+    <t>12/09/2022</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Cần thêm thành viên tham gia&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1</t>
   </si>
 </sst>
 </file>
@@ -535,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B357BE-472C-4729-B72D-D70006B2101F}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I16" sqref="I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -583,7 +584,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>10</v>
@@ -591,7 +592,7 @@
       <c r="C2" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="0" t="s">
@@ -611,6 +612,483 @@
       </c>
       <c r="J2" s="0" t="s">
         <v>15</v>
+      </c>
+      <c r="K2" s="0">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="0">
+        <v>3</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" s="0">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="0">
+        <v>4</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="0">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0">
+        <v>5</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G5" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H5" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="0">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0">
+        <v>6</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G6" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H6" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0">
+        <v>7</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F7" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G7" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H7" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="K7" s="0">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="0">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0">
+        <v>9</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="K9" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="0">
+        <v>10</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="1">
+        <v>44566</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J10" s="0">
+        <v>5</v>
+      </c>
+      <c r="K10" s="0">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="0">
+        <v>11</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1">
+        <v>44565</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H11" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="0">
+        <v>4</v>
+      </c>
+      <c r="K11" s="0">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="0">
+        <v>12</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="1">
+        <v>44564</v>
+      </c>
+      <c r="E12" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J12" s="0">
+        <v>3</v>
+      </c>
+      <c r="K12" s="0">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="0">
+        <v>13</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="1">
+        <v>44563</v>
+      </c>
+      <c r="E13" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="J13" s="0">
+        <v>2</v>
+      </c>
+      <c r="K13" s="0">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:K13">
+    <sortCondition ref="A1:A13" descending="1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A5329B-D34B-4AC3-89BA-839CA231C8DF}">
+  <dimension ref="A1:J14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="2" max="3" width="26.6640625" customWidth="1"/>
+    <col min="4" max="4" width="12.53125" customWidth="1"/>
+    <col min="5" max="5" width="17.53125" customWidth="1"/>
+    <col min="9" max="9" width="13.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="0" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="0">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G2" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H2" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3">
@@ -618,28 +1096,28 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>16</v>
+        <v>41</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1">
         <v>44563</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>19</v>
+        <v>42</v>
       </c>
       <c r="J3" s="0">
         <v>2</v>
@@ -650,25 +1128,25 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1">
         <v>44564</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I4" s="0" t="s">
         <v>14</v>
@@ -682,28 +1160,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D5" s="1">
         <v>44565</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="J5" s="0">
         <v>4</v>
@@ -714,28 +1192,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D6" s="1">
         <v>44566</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="J6" s="0">
         <v>5</v>
@@ -746,31 +1224,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="D7" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8">
@@ -778,31 +1256,31 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="D8" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9">
@@ -810,31 +1288,31 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>11</v>
-      </c>
       <c r="D9" s="0" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H9" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="0" t="s">
         <v>30</v>
-      </c>
-      <c r="F9" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="G9" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="H9" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="10">
@@ -842,16 +1320,16 @@
         <v>10</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="F10" s="0" t="b">
         <v>0</v>
@@ -866,7 +1344,7 @@
         <v>14</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11">
@@ -874,16 +1352,16 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>32</v>
+        <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="F11" s="0" t="b">
         <v>0</v>
@@ -898,7 +1376,7 @@
         <v>14</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12">
@@ -906,16 +1384,16 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F12" s="0" t="b">
         <v>0</v>
@@ -930,7 +1408,7 @@
         <v>14</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13">
@@ -938,16 +1416,16 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>42</v>
+        <v>16</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>43</v>
+        <v>17</v>
       </c>
       <c r="F13" s="0" t="b">
         <v>0</v>
@@ -962,7 +1440,7 @@
         <v>14</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>44</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14">
@@ -970,16 +1448,16 @@
         <v>14</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>33</v>
+        <v>12</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="F14" s="0" t="b">
         <v>0</v>
@@ -994,7 +1472,7 @@
         <v>14</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>38</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gửi duyệt quy trình + Sửa các lỗi khi không điền Input
</commit_message>
<xml_diff>
--- a/Hethongquanlylab/wwwroot/data/procedure.xlsx
+++ b/Hethongquanlylab/wwwroot/data/procedure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\C#\Hethongquanlylab\Hethongquanlylab\wwwroot\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F789E380-2636-4AC5-A249-98583EB3E4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3C21A9-E337-4488-B387-90B343500C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10996" xr2:uid="{C9AB2BF0-DA74-4C36-9550-9AB44C18DC50}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>id</t>
   </si>
@@ -110,25 +110,13 @@
     <t>&lt;p style="text-align: center;"&gt;&lt;span style="color: rgb(255, 0, 0);"&gt;Đây là quy trình rất quan trọng&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
+    <t>Quy trình đào tạo</t>
+  </si>
+  <si>
     <t>BanNhanSu</t>
   </si>
   <si>
-    <t>&lt;p&gt;Ngày 20/8/2022, Lab thầy Sinh tổ chức offline Lab tại trụ sở Tư Đình, Long Biên, Hà Nội&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>2hfsdjfhjkadfhads</t>
-  </si>
-  <si>
-    <t>Quy trình đào tạo</t>
-  </si>
-  <si>
     <t>09/09/2022</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong style="font-size: 11px;"&gt;&lt;em style="font-size: 30px; color: rgb(255, 0, 0);"&gt;adsadsadsa&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>1234</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;p&gt;&lt;strong style="font-size: 18px;"&gt;Đây là quy trình đào tạo&lt;/strong&gt;&lt;/p&gt;&lt;table style="border-collapse:collapse;width: 100%;"&gt;&lt;tbody&gt;_x000D_
@@ -164,25 +152,52 @@
     <t>Quy trình gặp 1-1</t>
   </si>
   <si>
+    <t>345</t>
+  </si>
+  <si>
+    <t>12/09/2022</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Cần thêm thành viên tham gia&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>https://developer.mozilla.org/en-US/docs/Web/HTML/Element/input</t>
+  </si>
+  <si>
+    <t>Đề án cuộc thi NCKH</t>
+  </si>
+  <si>
+    <t>https://www.plus2net.com4</t>
+  </si>
+  <si>
     <t>Đề án cuộc thi sáng tạo trẻ</t>
   </si>
   <si>
-    <t>Đề án cuộc thi NCKH</t>
-  </si>
-  <si>
-    <t>Trả lại</t>
-  </si>
-  <si>
-    <t>Quy trình tuyển 5.3t5345678</t>
-  </si>
-  <si>
-    <t>12/09/2022</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Cần thêm thành viên tham gia&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>1</t>
+    <t>01/03/2022 12:00:00 AM</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong style="font-size: 11px;"&gt;&lt;em style="font-size: 30px; color: rgb(255, 0, 0);"&gt;adsadsadsa&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ngày 20/8/2022, Lab thầy Sinh tổ chức offline Lab tại trụ sở Tư Đình, Long Biên, Hà Nội&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>2hfsdjfhjkadfhads</t>
+  </si>
+  <si>
+    <t>231</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/</t>
   </si>
 </sst>
 </file>
@@ -536,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16B357BE-472C-4729-B72D-D70006B2101F}">
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -727,34 +742,34 @@
         <v>6</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="G6" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="H6" s="0" t="b">
-        <v>0</v>
+        <v>27</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H6" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="K6" s="0">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7">
@@ -762,34 +777,34 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="G7" s="0" t="b">
-        <v>0</v>
-      </c>
-      <c r="H7" s="0" t="b">
-        <v>0</v>
+        <v>30</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="0" t="s">
+        <v>28</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K7" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
@@ -797,34 +812,34 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D8" s="1">
+        <v>44566</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="J8" s="0">
+        <v>5</v>
       </c>
       <c r="K8" s="0">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -832,34 +847,34 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <v>44565</v>
       </c>
       <c r="E9" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H9" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I9" s="0" t="s">
         <v>34</v>
       </c>
-      <c r="F9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H9" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I9" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J9" s="0" t="s">
-        <v>35</v>
+      <c r="J9" s="0">
+        <v>4</v>
       </c>
       <c r="K9" s="0">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -870,31 +885,31 @@
         <v>36</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1">
-        <v>44566</v>
+        <v>25</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>32</v>
+        <v>38</v>
+      </c>
+      <c r="F10" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G10" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H10" s="0" t="b">
+        <v>0</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J10" s="0">
-        <v>5</v>
+        <v>14</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="K10" s="0">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -902,34 +917,34 @@
         <v>11</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1">
-        <v>44565</v>
+        <v>25</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F11" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0" t="b">
+        <v>0</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="J11" s="0">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="K11" s="0">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -937,31 +952,31 @@
         <v>12</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="1">
-        <v>44564</v>
+        <v>25</v>
+      </c>
+      <c r="D12" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F12" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G12" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H12" s="0" t="b">
+        <v>0</v>
       </c>
       <c r="I12" s="0" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="0">
-        <v>3</v>
+      <c r="J12" s="0" t="s">
+        <v>44</v>
       </c>
       <c r="K12" s="0">
         <v>3</v>
@@ -972,39 +987,109 @@
         <v>13</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="1">
-        <v>44563</v>
+        <v>25</v>
+      </c>
+      <c r="D13" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="0" t="s">
-        <v>32</v>
+        <v>45</v>
+      </c>
+      <c r="F13" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G13" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H13" s="0" t="b">
+        <v>0</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J13" s="0">
-        <v>2</v>
+        <v>14</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="K13" s="0">
-        <v>2</v>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="0">
+        <v>14</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D14" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="F14" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G14" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H14" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I14" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="0">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>15</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="F15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="0">
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:K13">
-    <sortCondition ref="A1:A13" descending="1"/>
+    <sortCondition descending="1" ref="A1:A13"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
@@ -1013,7 +1098,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87A5329B-D34B-4AC3-89BA-839CA231C8DF}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
@@ -1064,16 +1149,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F2" s="0" t="b">
         <v>0</v>
@@ -1085,10 +1170,10 @@
         <v>0</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3">
@@ -1096,31 +1181,31 @@
         <v>2</v>
       </c>
       <c r="B3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="F3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H3" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3" s="0" t="s">
         <v>41</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="1">
-        <v>44563</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="J3" s="0">
-        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -1128,31 +1213,31 @@
         <v>3</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="1">
-        <v>44564</v>
+        <v>25</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
+      </c>
+      <c r="F4" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H4" s="0" t="b">
+        <v>0</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" s="0">
-        <v>3</v>
+        <v>34</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="5">
@@ -1160,28 +1245,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D5" s="1">
         <v>44565</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J5" s="0">
         <v>4</v>
@@ -1192,28 +1277,28 @@
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D6" s="1">
         <v>44566</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="J6" s="0">
         <v>5</v>
@@ -1224,31 +1309,31 @@
         <v>7</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I7" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8">
@@ -1256,31 +1341,31 @@
         <v>8</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="0" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>31</v>
-      </c>
       <c r="F8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I8" s="0" t="s">
         <v>14</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9">
@@ -1288,16 +1373,16 @@
         <v>9</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="F9" s="0" t="b">
         <v>0</v>
@@ -1309,10 +1394,10 @@
         <v>0</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10">
@@ -1323,13 +1408,13 @@
         <v>22</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D10" s="0" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="F10" s="0" t="b">
         <v>0</v>
@@ -1341,10 +1426,10 @@
         <v>0</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
@@ -1355,7 +1440,7 @@
         <v>22</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>25</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>12</v>
@@ -1373,7 +1458,7 @@
         <v>0</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J11" s="0" t="s">
         <v>15</v>
@@ -1473,6 +1558,38 @@
       </c>
       <c r="J14" s="0" t="s">
         <v>15</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="0">
+        <v>15</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="F15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="G15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="H15" s="0" t="b">
+        <v>0</v>
+      </c>
+      <c r="I15" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1482,6 +1599,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DFDF69E2F25F1C4A80F0FEAA8138CCDB" ma:contentTypeVersion="9" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="fe923e70f648911530141ebfdc9a4882">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2860ae03-02bd-455e-97e5-3bb4897f97b1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9171fb11caf7050feadfe5740d9471f9" ns3:_="">
     <xsd:import namespace="2860ae03-02bd-455e-97e5-3bb4897f97b1"/>
@@ -1657,35 +1789,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5506B35D-7100-472A-8546-075AD64EB5C0}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC5E854-D858-439B-BCEB-E443416E5990}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2860ae03-02bd-455e-97e5-3bb4897f97b1"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1707,9 +1814,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5DC5E854-D858-439B-BCEB-E443416E5990}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5506B35D-7100-472A-8546-075AD64EB5C0}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2860ae03-02bd-455e-97e5-3bb4897f97b1"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>